<commit_message>
agenda meeting 4, notule meeting 4, added audio meeting 4
+- agenda meeting 4
+ notule meeting 4
+ audio meeting 4
</commit_message>
<xml_diff>
--- a/Documentation/Documentation_made/vergaderingen/agenda_vergadering4.xlsx
+++ b/Documentation/Documentation_made/vergaderingen/agenda_vergadering4.xlsx
@@ -1,33 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18431"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\d2106\Documents\niv4\2017-2018\project\Barroc-IT-Groep-2\Documentation\Documentation_made\vergaderingen\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Youssef\Documents\GitKraken\Barroc-IT-Groep-2\Documentation\Documentation_made\vergaderingen\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="96" windowWidth="19440" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="90" windowWidth="19440" windowHeight="11760"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
     <sheet name="Blad2" sheetId="2" r:id="rId2"/>
     <sheet name="Blad3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Fer</author>
     <author>Fer Krimpen</author>
   </authors>
   <commentList>
-    <comment ref="E3" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
+    <comment ref="E3" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -51,7 +51,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B4" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
+    <comment ref="B4" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -75,7 +75,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H18" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0000-000003000000}">
+    <comment ref="H18" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -99,7 +99,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H19" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000004000000}">
+    <comment ref="H19" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -208,19 +208,19 @@
     <t>waar staan we</t>
   </si>
   <si>
-    <t>Datum: 25 sep 2017</t>
-  </si>
-  <si>
     <t>front-end</t>
   </si>
   <si>
     <t>back-end</t>
+  </si>
+  <si>
+    <t>Datum: 5 okt 2017</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="d\ mmmm\ yyyy"/>
   </numFmts>
@@ -537,40 +537,7 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="20" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -653,6 +620,39 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="20" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -674,7 +674,7 @@
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Kantoorthema">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Kantoor">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -712,7 +712,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Kantoor">
       <a:majorFont>
         <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -747,23 +747,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -799,26 +782,9 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Kantoor">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -991,507 +957,507 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:L60"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="B5" sqref="B5:D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.88671875" style="5" customWidth="1"/>
-    <col min="2" max="2" width="9.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="4.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5.88671875" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.88671875" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="2.85546875" style="5" customWidth="1"/>
+    <col min="2" max="2" width="9.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="4.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.85546875" style="4" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="77" style="5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.33203125" style="5" customWidth="1"/>
-    <col min="8" max="8" width="34.44140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="2.6640625" style="5" customWidth="1"/>
-    <col min="10" max="10" width="5.5546875" style="5" customWidth="1"/>
-    <col min="11" max="15" width="8.88671875" style="5"/>
+    <col min="7" max="7" width="7.28515625" style="5" customWidth="1"/>
+    <col min="8" max="8" width="34.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="2.7109375" style="5" customWidth="1"/>
+    <col min="10" max="10" width="5.5703125" style="5" customWidth="1"/>
+    <col min="11" max="15" width="8.85546875" style="5"/>
     <col min="16" max="16" width="22" style="5" customWidth="1"/>
-    <col min="17" max="16384" width="8.88671875" style="5"/>
+    <col min="17" max="16384" width="8.85546875" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="6"/>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="7"/>
-      <c r="G2" s="7"/>
-      <c r="H2" s="8"/>
-      <c r="I2" s="9"/>
-    </row>
-    <row r="3" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B3" s="10" t="s">
+    <row r="1" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="59"/>
+      <c r="C2" s="60"/>
+      <c r="D2" s="60"/>
+      <c r="E2" s="60"/>
+      <c r="F2" s="60"/>
+      <c r="G2" s="60"/>
+      <c r="H2" s="61"/>
+      <c r="I2" s="6"/>
+    </row>
+    <row r="3" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B3" s="62" t="s">
         <v>22</v>
       </c>
-      <c r="C3" s="11"/>
-      <c r="D3" s="12"/>
-      <c r="E3" s="13" t="s">
+      <c r="C3" s="63"/>
+      <c r="D3" s="64"/>
+      <c r="E3" s="65" t="s">
         <v>23</v>
       </c>
-      <c r="F3" s="14"/>
-      <c r="G3" s="14"/>
-      <c r="H3" s="15"/>
-      <c r="I3" s="9"/>
-    </row>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B4" s="16" t="s">
+      <c r="F3" s="66"/>
+      <c r="G3" s="66"/>
+      <c r="H3" s="67"/>
+      <c r="I3" s="6"/>
+    </row>
+    <row r="4" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B4" s="74" t="s">
         <v>24</v>
       </c>
-      <c r="C4" s="17"/>
-      <c r="D4" s="18"/>
-      <c r="E4" s="19"/>
-      <c r="F4" s="20"/>
-      <c r="G4" s="20"/>
-      <c r="H4" s="21"/>
-      <c r="I4" s="9"/>
-    </row>
-    <row r="5" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="22" t="s">
+      <c r="C4" s="75"/>
+      <c r="D4" s="76"/>
+      <c r="E4" s="68"/>
+      <c r="F4" s="69"/>
+      <c r="G4" s="69"/>
+      <c r="H4" s="70"/>
+      <c r="I4" s="6"/>
+    </row>
+    <row r="5" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="77" t="s">
+        <v>28</v>
+      </c>
+      <c r="C5" s="78"/>
+      <c r="D5" s="79"/>
+      <c r="E5" s="71"/>
+      <c r="F5" s="72"/>
+      <c r="G5" s="72"/>
+      <c r="H5" s="73"/>
+      <c r="I5" s="6"/>
+    </row>
+    <row r="6" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="E6" s="9"/>
+      <c r="F6" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="G6" s="11"/>
+      <c r="H6" s="12"/>
+      <c r="I6" s="6"/>
+    </row>
+    <row r="7" spans="2:10" ht="18" x14ac:dyDescent="0.25">
+      <c r="B7" s="13"/>
+      <c r="C7" s="14"/>
+      <c r="D7" s="15"/>
+      <c r="E7" s="16"/>
+      <c r="F7" s="17"/>
+      <c r="G7" s="18"/>
+      <c r="H7" s="19"/>
+      <c r="I7" s="20"/>
+    </row>
+    <row r="8" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B8" s="14"/>
+      <c r="C8" s="14">
+        <v>5</v>
+      </c>
+      <c r="D8" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="E8" s="16">
+        <v>1</v>
+      </c>
+      <c r="F8" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="G8" s="18"/>
+      <c r="H8" s="19"/>
+      <c r="I8" s="20"/>
+      <c r="J8" s="22"/>
+    </row>
+    <row r="9" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B9" s="14"/>
+      <c r="C9" s="14">
+        <v>2</v>
+      </c>
+      <c r="D9" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="E9" s="16">
+        <v>2</v>
+      </c>
+      <c r="F9" s="23" t="s">
+        <v>6</v>
+      </c>
+      <c r="H9" s="19"/>
+      <c r="I9" s="20"/>
+    </row>
+    <row r="10" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B10" s="14"/>
+      <c r="C10" s="14"/>
+      <c r="D10" s="24" t="s">
+        <v>5</v>
+      </c>
+      <c r="E10" s="16">
+        <v>3</v>
+      </c>
+      <c r="F10" s="23" t="s">
+        <v>20</v>
+      </c>
+      <c r="G10" s="18"/>
+      <c r="H10" s="19"/>
+      <c r="I10" s="20"/>
+    </row>
+    <row r="11" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B11" s="14"/>
+      <c r="C11" s="14">
+        <v>10</v>
+      </c>
+      <c r="D11" s="24"/>
+      <c r="E11" s="16">
+        <v>4</v>
+      </c>
+      <c r="F11" s="25" t="s">
+        <v>25</v>
+      </c>
+      <c r="G11" s="26"/>
+      <c r="H11" s="27"/>
+      <c r="I11" s="20"/>
+    </row>
+    <row r="12" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B12" s="14"/>
+      <c r="C12" s="14">
+        <v>10</v>
+      </c>
+      <c r="D12" s="24"/>
+      <c r="E12" s="16">
+        <v>5</v>
+      </c>
+      <c r="F12" s="28" t="s">
         <v>26</v>
       </c>
-      <c r="C5" s="23"/>
-      <c r="D5" s="24"/>
-      <c r="E5" s="25"/>
-      <c r="F5" s="26"/>
-      <c r="G5" s="26"/>
-      <c r="H5" s="27"/>
-      <c r="I5" s="9"/>
-    </row>
-    <row r="6" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="28" t="s">
-        <v>0</v>
-      </c>
-      <c r="C6" s="29" t="s">
+      <c r="G12" s="26"/>
+      <c r="H12" s="27"/>
+      <c r="I12" s="20"/>
+    </row>
+    <row r="13" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B13" s="14"/>
+      <c r="C13" s="14">
+        <v>5</v>
+      </c>
+      <c r="D13" s="24"/>
+      <c r="E13" s="16">
+        <v>6</v>
+      </c>
+      <c r="F13" s="28" t="s">
+        <v>27</v>
+      </c>
+      <c r="G13" s="26"/>
+      <c r="H13" s="27"/>
+      <c r="I13" s="20"/>
+    </row>
+    <row r="14" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B14" s="14"/>
+      <c r="C14" s="14"/>
+      <c r="D14" s="24"/>
+      <c r="E14" s="16">
+        <v>7</v>
+      </c>
+      <c r="G14" s="26"/>
+      <c r="H14" s="27"/>
+      <c r="I14" s="20"/>
+    </row>
+    <row r="15" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B15" s="14"/>
+      <c r="C15" s="14">
         <v>1</v>
       </c>
-      <c r="D6" s="29" t="s">
-        <v>2</v>
-      </c>
-      <c r="E6" s="30"/>
-      <c r="F6" s="31" t="s">
-        <v>3</v>
-      </c>
-      <c r="G6" s="32"/>
-      <c r="H6" s="33"/>
-      <c r="I6" s="9"/>
-    </row>
-    <row r="7" spans="2:10" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="B7" s="34"/>
-      <c r="C7" s="35"/>
-      <c r="D7" s="36"/>
-      <c r="E7" s="37"/>
-      <c r="F7" s="38"/>
-      <c r="G7" s="39"/>
-      <c r="H7" s="40"/>
-      <c r="I7" s="41"/>
-    </row>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B8" s="35"/>
-      <c r="C8" s="35">
+      <c r="D15" s="24" t="s">
+        <v>4</v>
+      </c>
+      <c r="E15" s="16">
+        <v>8</v>
+      </c>
+      <c r="F15" s="29" t="s">
+        <v>19</v>
+      </c>
+      <c r="G15" s="18"/>
+      <c r="H15" s="19"/>
+      <c r="I15" s="20"/>
+    </row>
+    <row r="16" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B16" s="24"/>
+      <c r="C16" s="14">
         <v>5</v>
       </c>
-      <c r="D8" s="35" t="s">
+      <c r="D16" s="24" t="s">
+        <v>5</v>
+      </c>
+      <c r="E16" s="16">
+        <v>9</v>
+      </c>
+      <c r="F16" s="30" t="s">
+        <v>9</v>
+      </c>
+      <c r="G16" s="18"/>
+      <c r="H16" s="19"/>
+      <c r="I16" s="20"/>
+    </row>
+    <row r="17" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B17" s="31"/>
+      <c r="C17" s="31"/>
+      <c r="D17" s="31"/>
+      <c r="E17" s="32"/>
+      <c r="F17" s="33"/>
+      <c r="G17" s="34"/>
+      <c r="H17" s="35"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B18" s="36"/>
+      <c r="C18" s="37"/>
+      <c r="D18" s="38" t="s">
+        <v>7</v>
+      </c>
+      <c r="E18" s="39" t="s">
+        <v>10</v>
+      </c>
+      <c r="F18" s="40"/>
+      <c r="G18" s="40"/>
+      <c r="H18" s="41" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B19" s="42"/>
+      <c r="C19" s="37"/>
+      <c r="D19" s="43" t="s">
+        <v>8</v>
+      </c>
+      <c r="E19" s="39" t="s">
+        <v>11</v>
+      </c>
+      <c r="F19" s="44"/>
+      <c r="G19" s="44"/>
+      <c r="H19" s="41"/>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B20" s="42"/>
+      <c r="C20" s="37"/>
+      <c r="D20" s="43" t="s">
+        <v>5</v>
+      </c>
+      <c r="E20" s="39" t="s">
+        <v>12</v>
+      </c>
+      <c r="F20" s="44"/>
+      <c r="G20" s="44"/>
+      <c r="H20" s="45"/>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B21" s="42"/>
+      <c r="C21" s="37"/>
+      <c r="D21" s="43" t="s">
         <v>13</v>
       </c>
-      <c r="E8" s="37">
-        <v>1</v>
-      </c>
-      <c r="F8" s="42" t="s">
-        <v>18</v>
-      </c>
-      <c r="G8" s="39"/>
-      <c r="H8" s="40"/>
-      <c r="I8" s="41"/>
-      <c r="J8" s="43"/>
-    </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B9" s="35"/>
-      <c r="C9" s="35">
-        <v>2</v>
-      </c>
-      <c r="D9" s="35" t="s">
-        <v>13</v>
-      </c>
-      <c r="E9" s="37">
-        <v>2</v>
-      </c>
-      <c r="F9" s="44" t="s">
-        <v>6</v>
-      </c>
-      <c r="H9" s="40"/>
-      <c r="I9" s="41"/>
-    </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B10" s="35"/>
-      <c r="C10" s="35"/>
-      <c r="D10" s="45" t="s">
-        <v>5</v>
-      </c>
-      <c r="E10" s="37">
-        <v>3</v>
-      </c>
-      <c r="F10" s="44" t="s">
-        <v>20</v>
-      </c>
-      <c r="G10" s="39"/>
-      <c r="H10" s="40"/>
-      <c r="I10" s="41"/>
-    </row>
-    <row r="11" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B11" s="35"/>
-      <c r="C11" s="35">
-        <v>10</v>
-      </c>
-      <c r="D11" s="45"/>
-      <c r="E11" s="37">
+      <c r="E21" s="39" t="s">
+        <v>14</v>
+      </c>
+      <c r="F21" s="44"/>
+      <c r="G21" s="44"/>
+      <c r="H21" s="45"/>
+    </row>
+    <row r="22" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B22" s="46"/>
+      <c r="C22" s="47"/>
+      <c r="D22" s="48" t="s">
         <v>4</v>
       </c>
-      <c r="F11" s="46" t="s">
-        <v>25</v>
-      </c>
-      <c r="G11" s="47"/>
-      <c r="H11" s="48"/>
-      <c r="I11" s="41"/>
-    </row>
-    <row r="12" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B12" s="35"/>
-      <c r="C12" s="35">
-        <v>10</v>
-      </c>
-      <c r="D12" s="45"/>
-      <c r="E12" s="37">
-        <v>5</v>
-      </c>
-      <c r="F12" s="49" t="s">
-        <v>27</v>
-      </c>
-      <c r="G12" s="47"/>
-      <c r="H12" s="48"/>
-      <c r="I12" s="41"/>
-    </row>
-    <row r="13" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B13" s="35"/>
-      <c r="C13" s="35">
-        <v>5</v>
-      </c>
-      <c r="D13" s="45"/>
-      <c r="E13" s="37">
-        <v>6</v>
-      </c>
-      <c r="F13" s="49" t="s">
-        <v>28</v>
-      </c>
-      <c r="G13" s="47"/>
-      <c r="H13" s="48"/>
-      <c r="I13" s="41"/>
-    </row>
-    <row r="14" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B14" s="35"/>
-      <c r="C14" s="35"/>
-      <c r="D14" s="45"/>
-      <c r="E14" s="37">
-        <v>7</v>
-      </c>
-      <c r="G14" s="47"/>
-      <c r="H14" s="48"/>
-      <c r="I14" s="41"/>
-    </row>
-    <row r="15" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B15" s="35"/>
-      <c r="C15" s="35">
-        <v>1</v>
-      </c>
-      <c r="D15" s="45" t="s">
-        <v>4</v>
-      </c>
-      <c r="E15" s="37">
-        <v>8</v>
-      </c>
-      <c r="F15" s="50" t="s">
-        <v>19</v>
-      </c>
-      <c r="G15" s="39"/>
-      <c r="H15" s="40"/>
-      <c r="I15" s="41"/>
-    </row>
-    <row r="16" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B16" s="45"/>
-      <c r="C16" s="35">
-        <v>5</v>
-      </c>
-      <c r="D16" s="45" t="s">
-        <v>5</v>
-      </c>
-      <c r="E16" s="37">
-        <v>9</v>
-      </c>
-      <c r="F16" s="51" t="s">
-        <v>9</v>
-      </c>
-      <c r="G16" s="39"/>
-      <c r="H16" s="40"/>
-      <c r="I16" s="41"/>
-    </row>
-    <row r="17" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B17" s="52"/>
-      <c r="C17" s="52"/>
-      <c r="D17" s="52"/>
-      <c r="E17" s="53"/>
-      <c r="F17" s="54"/>
-      <c r="G17" s="55"/>
-      <c r="H17" s="56"/>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B18" s="57"/>
-      <c r="C18" s="58"/>
-      <c r="D18" s="59" t="s">
-        <v>7</v>
-      </c>
-      <c r="E18" s="60" t="s">
-        <v>10</v>
-      </c>
-      <c r="F18" s="61"/>
-      <c r="G18" s="61"/>
-      <c r="H18" s="62" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B19" s="63"/>
-      <c r="C19" s="58"/>
-      <c r="D19" s="64" t="s">
-        <v>8</v>
-      </c>
-      <c r="E19" s="60" t="s">
-        <v>11</v>
-      </c>
-      <c r="F19" s="65"/>
-      <c r="G19" s="65"/>
-      <c r="H19" s="62"/>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B20" s="63"/>
-      <c r="C20" s="58"/>
-      <c r="D20" s="64" t="s">
-        <v>5</v>
-      </c>
-      <c r="E20" s="60" t="s">
-        <v>12</v>
-      </c>
-      <c r="F20" s="65"/>
-      <c r="G20" s="65"/>
-      <c r="H20" s="66"/>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B21" s="63"/>
-      <c r="C21" s="58"/>
-      <c r="D21" s="64" t="s">
-        <v>13</v>
-      </c>
-      <c r="E21" s="60" t="s">
-        <v>14</v>
-      </c>
-      <c r="F21" s="65"/>
-      <c r="G21" s="65"/>
-      <c r="H21" s="66"/>
-    </row>
-    <row r="22" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B22" s="67"/>
-      <c r="C22" s="68"/>
-      <c r="D22" s="69" t="s">
-        <v>4</v>
-      </c>
-      <c r="E22" s="70" t="s">
+      <c r="E22" s="49" t="s">
         <v>15</v>
       </c>
-      <c r="F22" s="71"/>
-      <c r="G22" s="71"/>
-      <c r="H22" s="72"/>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="F22" s="50"/>
+      <c r="G22" s="50"/>
+      <c r="H22" s="51"/>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E24" s="4" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B25" s="73"/>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B25" s="52"/>
       <c r="E25" s="4">
         <v>1</v>
       </c>
-      <c r="F25" s="74"/>
-      <c r="I25" s="75"/>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="F25" s="53"/>
+      <c r="I25" s="54"/>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C26" s="1"/>
       <c r="E26" s="4">
         <v>2</v>
       </c>
-      <c r="F26" s="76"/>
-      <c r="I26" s="75"/>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="F26" s="55"/>
+      <c r="I26" s="54"/>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C27" s="1"/>
       <c r="E27" s="4">
         <v>3</v>
       </c>
-      <c r="F27" s="76"/>
-      <c r="I27" s="75"/>
-    </row>
-    <row r="28" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="F27" s="55"/>
+      <c r="I27" s="54"/>
+    </row>
+    <row r="28" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="5"/>
       <c r="D28" s="3"/>
       <c r="E28" s="4">
         <v>4</v>
       </c>
-      <c r="F28" s="76"/>
-      <c r="G28" s="77"/>
-      <c r="H28" s="77"/>
-      <c r="I28" s="78"/>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="F28" s="55"/>
+      <c r="G28" s="56"/>
+      <c r="H28" s="56"/>
+      <c r="I28" s="57"/>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="1"/>
       <c r="E29" s="4">
         <v>5</v>
       </c>
-      <c r="I29" s="75"/>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="I29" s="54"/>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="1"/>
       <c r="E30" s="4">
         <v>6</v>
       </c>
-      <c r="F30" s="74"/>
-      <c r="I30" s="75"/>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="F30" s="53"/>
+      <c r="I30" s="54"/>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
       <c r="E31" s="4">
         <v>7</v>
       </c>
-      <c r="F31" s="74"/>
-      <c r="I31" s="75"/>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="F31" s="53"/>
+      <c r="I31" s="54"/>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" s="1"/>
-      <c r="F32" s="74"/>
-      <c r="I32" s="75"/>
-    </row>
-    <row r="33" spans="5:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F32" s="53"/>
+      <c r="I32" s="54"/>
+    </row>
+    <row r="33" spans="5:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E33" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="I33" s="75"/>
-    </row>
-    <row r="34" spans="5:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="I33" s="54"/>
+    </row>
+    <row r="34" spans="5:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E34" s="4">
         <v>1</v>
       </c>
-      <c r="F34" s="79"/>
-      <c r="I34" s="75"/>
-      <c r="J34" s="79"/>
-      <c r="K34" s="79"/>
-      <c r="L34" s="79"/>
-    </row>
-    <row r="35" spans="5:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F34" s="58"/>
+      <c r="I34" s="54"/>
+      <c r="J34" s="58"/>
+      <c r="K34" s="58"/>
+      <c r="L34" s="58"/>
+    </row>
+    <row r="35" spans="5:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E35" s="4">
         <v>2</v>
       </c>
-      <c r="F35" s="79"/>
-      <c r="I35" s="75"/>
-      <c r="J35" s="79"/>
-      <c r="K35" s="79"/>
-      <c r="L35" s="79"/>
-    </row>
-    <row r="36" spans="5:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F35" s="58"/>
+      <c r="I35" s="54"/>
+      <c r="J35" s="58"/>
+      <c r="K35" s="58"/>
+      <c r="L35" s="58"/>
+    </row>
+    <row r="36" spans="5:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E36" s="4">
         <v>3</v>
       </c>
-      <c r="I36" s="75"/>
-      <c r="J36" s="79"/>
-      <c r="K36" s="79"/>
-      <c r="L36" s="79"/>
-    </row>
-    <row r="37" spans="5:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="I37" s="9"/>
-    </row>
-    <row r="38" spans="5:12" ht="10.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="I38" s="9"/>
-    </row>
-    <row r="39" spans="5:12" ht="10.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="I39" s="9"/>
-    </row>
-    <row r="40" spans="5:12" ht="10.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="I40" s="9"/>
-    </row>
-    <row r="41" spans="5:12" ht="10.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="I41" s="9"/>
-    </row>
-    <row r="42" spans="5:12" ht="10.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="I42" s="9"/>
-    </row>
-    <row r="43" spans="5:12" x14ac:dyDescent="0.3">
-      <c r="I43" s="9"/>
-    </row>
-    <row r="44" spans="5:12" x14ac:dyDescent="0.3">
-      <c r="I44" s="9"/>
-    </row>
-    <row r="45" spans="5:12" x14ac:dyDescent="0.3">
-      <c r="I45" s="9"/>
-    </row>
-    <row r="46" spans="5:12" x14ac:dyDescent="0.3">
-      <c r="I46" s="9"/>
-    </row>
-    <row r="47" spans="5:12" x14ac:dyDescent="0.3">
-      <c r="I47" s="9"/>
-    </row>
-    <row r="48" spans="5:12" x14ac:dyDescent="0.3">
-      <c r="I48" s="9"/>
-    </row>
-    <row r="49" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I49" s="9"/>
-    </row>
-    <row r="50" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I50" s="9"/>
-    </row>
-    <row r="51" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I51" s="9"/>
-    </row>
-    <row r="52" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I52" s="9"/>
-    </row>
-    <row r="53" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I53" s="9"/>
-    </row>
-    <row r="54" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I54" s="9"/>
-    </row>
-    <row r="55" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I55" s="9"/>
-    </row>
-    <row r="56" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I56" s="9"/>
-    </row>
-    <row r="57" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I57" s="9"/>
-    </row>
-    <row r="58" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I58" s="9"/>
-    </row>
-    <row r="59" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I59" s="9"/>
-    </row>
-    <row r="60" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I60" s="9"/>
+      <c r="I36" s="54"/>
+      <c r="J36" s="58"/>
+      <c r="K36" s="58"/>
+      <c r="L36" s="58"/>
+    </row>
+    <row r="37" spans="5:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I37" s="6"/>
+    </row>
+    <row r="38" spans="5:12" ht="10.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I38" s="6"/>
+    </row>
+    <row r="39" spans="5:12" ht="10.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I39" s="6"/>
+    </row>
+    <row r="40" spans="5:12" ht="10.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I40" s="6"/>
+    </row>
+    <row r="41" spans="5:12" ht="10.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I41" s="6"/>
+    </row>
+    <row r="42" spans="5:12" ht="10.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I42" s="6"/>
+    </row>
+    <row r="43" spans="5:12" x14ac:dyDescent="0.25">
+      <c r="I43" s="6"/>
+    </row>
+    <row r="44" spans="5:12" x14ac:dyDescent="0.25">
+      <c r="I44" s="6"/>
+    </row>
+    <row r="45" spans="5:12" x14ac:dyDescent="0.25">
+      <c r="I45" s="6"/>
+    </row>
+    <row r="46" spans="5:12" x14ac:dyDescent="0.25">
+      <c r="I46" s="6"/>
+    </row>
+    <row r="47" spans="5:12" x14ac:dyDescent="0.25">
+      <c r="I47" s="6"/>
+    </row>
+    <row r="48" spans="5:12" x14ac:dyDescent="0.25">
+      <c r="I48" s="6"/>
+    </row>
+    <row r="49" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I49" s="6"/>
+    </row>
+    <row r="50" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I50" s="6"/>
+    </row>
+    <row r="51" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I51" s="6"/>
+    </row>
+    <row r="52" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I52" s="6"/>
+    </row>
+    <row r="53" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I53" s="6"/>
+    </row>
+    <row r="54" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I54" s="6"/>
+    </row>
+    <row r="55" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I55" s="6"/>
+    </row>
+    <row r="56" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I56" s="6"/>
+    </row>
+    <row r="57" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I57" s="6"/>
+    </row>
+    <row r="58" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I58" s="6"/>
+    </row>
+    <row r="59" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I59" s="6"/>
+    </row>
+    <row r="60" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I60" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -1508,24 +1474,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1581,18 +1547,18 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1611,6 +1577,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{56D4A539-5E71-46A4-A076-A8448D6640BC}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7EC78C7E-41AD-4518-BFAA-0ABA4B09AB48}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
@@ -1622,12 +1596,4 @@
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{56D4A539-5E71-46A4-A076-A8448D6640BC}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>